<commit_message>
removed the peak torque and pwoer graphs from the plots
</commit_message>
<xml_diff>
--- a/Sizing/motorData/motorData.xlsx
+++ b/Sizing/motorData/motorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ElectricMotors\Sizing\motorData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F305205D-B89D-4A59-9C5E-0900187392A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8CAF0E-C6D6-4A39-BE49-626F4E1E6E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="1215" windowWidth="19560" windowHeight="17520" tabRatio="800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="800" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brocheure" sheetId="25" r:id="rId1"/>
@@ -362,14 +362,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E489C59-36A1-477C-846B-9F91113B8F10}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -725,7 +725,7 @@
     <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>44</v>
       </c>
@@ -742,7 +742,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -762,7 +762,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -782,7 +782,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -801,8 +801,12 @@
       <c r="F4">
         <v>455</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4">
+        <f>E4*5</f>
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -822,7 +826,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -842,7 +846,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -862,7 +866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -882,27 +886,27 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>116</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <v>150</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>201</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>218</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -922,7 +926,7 @@
         <v>1570</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -942,31 +946,31 @@
         <v>4650</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="13">
         <v>95</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -986,7 +990,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1006,7 +1010,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1030,37 +1034,37 @@
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">
@@ -1083,23 +1087,23 @@
       <c r="A24" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="11">
         <f>B3*360/1000</f>
         <v>117.36</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <f>C3*360/1000</f>
         <v>157.32</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="11">
         <f>D3*360/1000</f>
         <v>199.44</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="11">
         <f>E3*360/1000</f>
         <v>230.76</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="11">
         <f>F3*360/1000</f>
         <v>183.96</v>
       </c>
@@ -1108,23 +1112,23 @@
       <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <f>B3*600/1000</f>
         <v>195.6</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <f>C3*600/1000</f>
         <v>262.2</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="11">
         <f>D3*600/1000</f>
         <v>332.4</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="11">
         <f>E3*600/1000</f>
         <v>384.6</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="11">
         <f>F3*600/1000</f>
         <v>306.60000000000002</v>
       </c>
@@ -1133,124 +1137,124 @@
       <c r="A26" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="11">
         <f>B11*B5*2*3.14/60/1000*0.95</f>
         <v>195.38649999999998</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <f t="shared" ref="C26:F26" si="0">C11*C5*2*3.14/60/1000*0.95</f>
         <v>245.79919999999998</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <f t="shared" si="0"/>
         <v>329.32319999999999</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="11">
         <f t="shared" si="0"/>
         <v>423.8843</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="11">
         <f t="shared" si="0"/>
         <v>515.07461000000001</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="2:6">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="2:6">
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="2:6">
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="2:6">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="2:6">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="2:6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -13711,8 +13715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16016,15 +16020,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a077bfdb5c83a9e90026d9660a1fda64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab75e0c3651772810f3079df645c8c4c" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -16229,6 +16224,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -16236,14 +16240,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C02CEFC-A583-411E-ADB9-AA231F4E5AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3A78C7F-AFE2-46DF-A32E-9F7304FDE51E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16262,6 +16258,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C02CEFC-A583-411E-ADB9-AA231F4E5AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5B302CA-2A32-4C0C-88B4-3C4E2975CF79}">
   <ds:schemaRefs>

</xml_diff>